<commit_message>
Docs - add paper docs & latest development
</commit_message>
<xml_diff>
--- a/Documents/Classeur1.xlsx
+++ b/Documents/Classeur1.xlsx
@@ -554,9 +554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -946,7 +944,7 @@
         <v>4096</v>
       </c>
       <c r="I20">
-        <f>SUM(H6:H20)</f>
+        <f t="shared" ref="I20:I34" si="1">SUM(H6:H20)</f>
         <v>4096</v>
       </c>
       <c r="J20" s="12">
@@ -954,7 +952,7 @@
         <v>273.06666666666666</v>
       </c>
       <c r="K20" s="12">
-        <f>J20+$I$2</f>
+        <f t="shared" ref="K20:K34" si="2">J20+$I$2</f>
         <v>33041.066666666666</v>
       </c>
     </row>
@@ -980,15 +978,15 @@
         <v>6144</v>
       </c>
       <c r="I21">
-        <f>SUM(H7:H21)</f>
+        <f t="shared" si="1"/>
         <v>10240</v>
       </c>
       <c r="J21" s="12">
-        <f t="shared" ref="J21:J34" si="1">I21/$I$3</f>
+        <f t="shared" ref="J21:J34" si="3">I21/$I$3</f>
         <v>682.66666666666663</v>
       </c>
       <c r="K21" s="12">
-        <f>J21+$I$2</f>
+        <f t="shared" si="2"/>
         <v>33450.666666666664</v>
       </c>
     </row>
@@ -1014,15 +1012,15 @@
         <v>8192</v>
       </c>
       <c r="I22">
-        <f>SUM(H8:H22)</f>
+        <f t="shared" si="1"/>
         <v>18432</v>
       </c>
       <c r="J22" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1228.8</v>
       </c>
       <c r="K22" s="12">
-        <f>J22+$I$2</f>
+        <f t="shared" si="2"/>
         <v>33996.800000000003</v>
       </c>
     </row>
@@ -1048,15 +1046,15 @@
         <v>10240</v>
       </c>
       <c r="I23">
-        <f>SUM(H9:H23)</f>
+        <f t="shared" si="1"/>
         <v>28672</v>
       </c>
       <c r="J23" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1911.4666666666667</v>
       </c>
       <c r="K23" s="12">
-        <f>J23+$I$2</f>
+        <f t="shared" si="2"/>
         <v>34679.466666666667</v>
       </c>
     </row>
@@ -1080,15 +1078,15 @@
         <v>12288</v>
       </c>
       <c r="I24">
-        <f>SUM(H10:H24)</f>
+        <f t="shared" si="1"/>
         <v>40960</v>
       </c>
       <c r="J24" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2730.6666666666665</v>
       </c>
       <c r="K24" s="12">
-        <f>J24+$I$2</f>
+        <f t="shared" si="2"/>
         <v>35498.666666666664</v>
       </c>
       <c r="Q24" s="12"/>
@@ -1104,7 +1102,7 @@
         <v>1.5</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" ref="E25:E35" si="2">C25+$D$3</f>
+        <f t="shared" ref="E25:E35" si="4">C25+$D$3</f>
         <v>38912</v>
       </c>
       <c r="F25" s="2">
@@ -1114,15 +1112,15 @@
         <v>14336</v>
       </c>
       <c r="I25">
-        <f>SUM(H11:H25)</f>
+        <f t="shared" si="1"/>
         <v>55296</v>
       </c>
       <c r="J25" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3686.4</v>
       </c>
       <c r="K25" s="12">
-        <f>J25+$I$2</f>
+        <f t="shared" si="2"/>
         <v>36454.400000000001</v>
       </c>
       <c r="Q25" s="12"/>
@@ -1138,7 +1136,7 @@
         <v>2</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40960</v>
       </c>
       <c r="F26" s="2">
@@ -1148,15 +1146,15 @@
         <v>16384</v>
       </c>
       <c r="I26">
-        <f>SUM(H12:H26)</f>
+        <f t="shared" si="1"/>
         <v>71680</v>
       </c>
       <c r="J26" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4778.666666666667</v>
       </c>
       <c r="K26" s="12">
-        <f>J26+$I$2</f>
+        <f t="shared" si="2"/>
         <v>37546.666666666664</v>
       </c>
       <c r="Q26" s="12"/>
@@ -1172,7 +1170,7 @@
         <v>2.5</v>
       </c>
       <c r="E27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>43008</v>
       </c>
       <c r="F27" s="2">
@@ -1182,15 +1180,15 @@
         <v>18432</v>
       </c>
       <c r="I27">
-        <f>SUM(H13:H27)</f>
+        <f t="shared" si="1"/>
         <v>90112</v>
       </c>
       <c r="J27" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6007.4666666666662</v>
       </c>
       <c r="K27" s="12">
-        <f>J27+$I$2</f>
+        <f t="shared" si="2"/>
         <v>38775.466666666667</v>
       </c>
       <c r="Q27" s="12"/>
@@ -1206,7 +1204,7 @@
         <v>3</v>
       </c>
       <c r="E28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>45056</v>
       </c>
       <c r="F28" s="2">
@@ -1216,15 +1214,15 @@
         <v>20480</v>
       </c>
       <c r="I28">
-        <f>SUM(H14:H28)</f>
+        <f t="shared" si="1"/>
         <v>110592</v>
       </c>
       <c r="J28" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7372.8</v>
       </c>
       <c r="K28" s="12">
-        <f>J28+$I$2</f>
+        <f t="shared" si="2"/>
         <v>40140.800000000003</v>
       </c>
       <c r="Q28" s="12"/>
@@ -1240,7 +1238,7 @@
         <v>3.5</v>
       </c>
       <c r="E29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>47104</v>
       </c>
       <c r="F29" s="2">
@@ -1250,15 +1248,15 @@
         <v>22528</v>
       </c>
       <c r="I29">
-        <f>SUM(H15:H29)</f>
+        <f t="shared" si="1"/>
         <v>133120</v>
       </c>
       <c r="J29" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8874.6666666666661</v>
       </c>
       <c r="K29" s="12">
-        <f>J29+$I$2</f>
+        <f t="shared" si="2"/>
         <v>41642.666666666664</v>
       </c>
       <c r="Q29" s="12"/>
@@ -1274,7 +1272,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>49152</v>
       </c>
       <c r="F30" s="2">
@@ -1284,15 +1282,15 @@
         <v>24576</v>
       </c>
       <c r="I30">
-        <f>SUM(H16:H30)</f>
+        <f t="shared" si="1"/>
         <v>157696</v>
       </c>
       <c r="J30" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10513.066666666668</v>
       </c>
       <c r="K30" s="12">
-        <f>J30+$I$2</f>
+        <f t="shared" si="2"/>
         <v>43281.066666666666</v>
       </c>
       <c r="Q30" s="12"/>
@@ -1308,7 +1306,7 @@
         <v>4.5</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>51200</v>
       </c>
       <c r="F31" s="2">
@@ -1318,15 +1316,15 @@
         <v>26624</v>
       </c>
       <c r="I31">
-        <f>SUM(H17:H31)</f>
+        <f t="shared" si="1"/>
         <v>184320</v>
       </c>
       <c r="J31" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>12288</v>
       </c>
       <c r="K31" s="12">
-        <f>J31+$I$2</f>
+        <f t="shared" si="2"/>
         <v>45056</v>
       </c>
       <c r="Q31" s="12"/>
@@ -1342,7 +1340,7 @@
         <v>5</v>
       </c>
       <c r="E32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>53248</v>
       </c>
       <c r="F32" s="2">
@@ -1352,15 +1350,15 @@
         <v>28672</v>
       </c>
       <c r="I32">
-        <f>SUM(H18:H32)</f>
+        <f t="shared" si="1"/>
         <v>212992</v>
       </c>
       <c r="J32" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>14199.466666666667</v>
       </c>
       <c r="K32" s="12">
-        <f>J32+$I$2</f>
+        <f t="shared" si="2"/>
         <v>46967.466666666667</v>
       </c>
       <c r="Q32" s="12"/>
@@ -1376,7 +1374,7 @@
         <v>5.5</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>55296</v>
       </c>
       <c r="F33" s="2">
@@ -1386,15 +1384,15 @@
         <v>30720</v>
       </c>
       <c r="I33">
-        <f>SUM(H19:H33)</f>
+        <f t="shared" si="1"/>
         <v>243712</v>
       </c>
       <c r="J33" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>16247.466666666667</v>
       </c>
       <c r="K33" s="12">
-        <f>J33+$I$2</f>
+        <f t="shared" si="2"/>
         <v>49015.466666666667</v>
       </c>
       <c r="Q33" s="12"/>
@@ -1410,7 +1408,7 @@
         <v>6</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>57344</v>
       </c>
       <c r="F34" s="2">
@@ -1420,15 +1418,15 @@
         <v>32767</v>
       </c>
       <c r="I34">
-        <f>SUM(H20:H34)</f>
+        <f t="shared" si="1"/>
         <v>276479</v>
       </c>
       <c r="J34" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>18431.933333333334</v>
       </c>
       <c r="K34" s="12">
-        <f>J34+$I$2</f>
+        <f t="shared" si="2"/>
         <v>51199.933333333334</v>
       </c>
       <c r="Q34" s="12"/>
@@ -1444,7 +1442,7 @@
         <v>6.5</v>
       </c>
       <c r="E35" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>59392</v>
       </c>
       <c r="F35" s="2">

</xml_diff>